<commit_message>
Cleaned up database issue - seems to be working.
</commit_message>
<xml_diff>
--- a/resources/db/Slated.xlsx
+++ b/resources/db/Slated.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="110">
   <si>
     <t>Case</t>
   </si>
@@ -35,9 +35,6 @@
   </si>
   <si>
     <t>Degree</t>
-  </si>
-  <si>
-    <t>21TRD09386</t>
   </si>
   <si>
     <t>21TRD09386-A</t>
@@ -792,7 +789,7 @@
   <dimension ref="A1:H24"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
@@ -824,579 +821,579 @@
         <v>6</v>
       </c>
       <c r="H1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A2" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="D2" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="E2" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="F2" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="G2" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="G2" s="1" t="s">
-        <v>13</v>
-      </c>
       <c r="H2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="38" x14ac:dyDescent="0.5">
       <c r="A3" s="1" t="s">
-        <v>7</v>
+        <v>109</v>
       </c>
       <c r="B3" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E3" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C3" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="E3" s="1" t="s">
+      <c r="F3" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="F3" s="1" t="s">
+      <c r="G3" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="G3" s="1" t="s">
-        <v>17</v>
-      </c>
       <c r="H3" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="50.7" x14ac:dyDescent="0.5">
       <c r="A4" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B4" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="C4" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="D4" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="E4" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="E4" s="1" t="s">
+      <c r="F4" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="F4" s="1" t="s">
-        <v>23</v>
-      </c>
       <c r="G4" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H4" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="50.7" x14ac:dyDescent="0.5">
       <c r="A5" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B5" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="C5" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="D5" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="D5" s="1" t="s">
+      <c r="E5" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="E5" s="1" t="s">
+      <c r="F5" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="F5" s="1" t="s">
+      <c r="G5" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="G5" s="1" t="s">
-        <v>30</v>
-      </c>
       <c r="H5" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="25.35" x14ac:dyDescent="0.5">
       <c r="A6" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B6" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="C6" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="C6" s="1" t="s">
+      <c r="D6" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="D6" s="1" t="s">
+      <c r="E6" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="E6" s="1" t="s">
+      <c r="F6" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="F6" s="1" t="s">
-        <v>36</v>
-      </c>
       <c r="G6" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H6" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="38" x14ac:dyDescent="0.5">
       <c r="A7" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B7" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="C7" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="C7" s="1" t="s">
+      <c r="D7" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="D7" s="1" t="s">
+      <c r="E7" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="E7" s="1" t="s">
+      <c r="F7" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="F7" s="1" t="s">
-        <v>42</v>
-      </c>
       <c r="G7" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H7" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="25.35" x14ac:dyDescent="0.5">
       <c r="A8" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B8" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="E8" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="C8" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="E8" s="1" t="s">
+      <c r="F8" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="F8" s="1" t="s">
-        <v>45</v>
-      </c>
       <c r="G8" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H8" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="25.35" x14ac:dyDescent="0.5">
       <c r="A9" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B9" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="E9" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="C9" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="E9" s="1" t="s">
+      <c r="F9" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="F9" s="1" t="s">
+      <c r="G9" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="G9" s="1" t="s">
-        <v>49</v>
-      </c>
       <c r="H9" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="38" x14ac:dyDescent="0.5">
       <c r="A10" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B10" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="B10" s="1" t="s">
+      <c r="C10" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="C10" s="1" t="s">
+      <c r="D10" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="D10" s="1" t="s">
+      <c r="E10" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="E10" s="1" t="s">
+      <c r="F10" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="F10" s="1" t="s">
-        <v>55</v>
-      </c>
       <c r="G10" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H10" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="11" spans="1:8" ht="50.7" x14ac:dyDescent="0.5">
       <c r="A11" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B11" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="B11" s="1" t="s">
+      <c r="C11" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="C11" s="1" t="s">
+      <c r="D11" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="D11" s="1" t="s">
+      <c r="E11" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="E11" s="1" t="s">
+      <c r="F11" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="F11" s="1" t="s">
+      <c r="G11" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="G11" s="1" t="s">
-        <v>62</v>
-      </c>
       <c r="H11" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="12" spans="1:8" ht="50.7" x14ac:dyDescent="0.5">
       <c r="A12" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="B12" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="B12" s="1" t="s">
+      <c r="C12" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="E12" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="C12" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="E12" s="1" t="s">
+      <c r="F12" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="F12" s="1" t="s">
-        <v>66</v>
-      </c>
       <c r="G12" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H12" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="13" spans="1:8" ht="38" x14ac:dyDescent="0.5">
       <c r="A13" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="B13" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="B13" s="1" t="s">
+      <c r="C13" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="C13" s="1" t="s">
+      <c r="D13" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="D13" s="1" t="s">
+      <c r="E13" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="E13" s="1" t="s">
+      <c r="F13" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="F13" s="1" t="s">
-        <v>72</v>
-      </c>
       <c r="G13" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="H13" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="14" spans="1:8" ht="25.35" x14ac:dyDescent="0.5">
       <c r="A14" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B14" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="B14" s="1" t="s">
+      <c r="C14" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="C14" s="1" t="s">
+      <c r="D14" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="D14" s="1" t="s">
-        <v>76</v>
-      </c>
       <c r="E14" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="F14" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="F14" s="1" t="s">
+      <c r="G14" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="G14" s="1" t="s">
-        <v>49</v>
-      </c>
       <c r="H14" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A15" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B15" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="E15" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="C15" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="D15" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="E15" s="1" t="s">
+      <c r="F15" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="F15" s="1" t="s">
-        <v>79</v>
-      </c>
       <c r="G15" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="H15" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="16" spans="1:8" ht="25.35" x14ac:dyDescent="0.5">
       <c r="A16" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B16" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="E16" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="C16" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="D16" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="E16" s="1" t="s">
+      <c r="F16" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="F16" s="1" t="s">
-        <v>82</v>
-      </c>
       <c r="G16" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H16" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A17" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="B17" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="B17" s="1" t="s">
+      <c r="C17" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="C17" s="1" t="s">
+      <c r="D17" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="D17" s="1" t="s">
-        <v>86</v>
-      </c>
       <c r="E17" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F17" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="F17" s="1" t="s">
+      <c r="G17" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="G17" s="1" t="s">
-        <v>13</v>
-      </c>
       <c r="H17" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="18" spans="1:8" ht="38" x14ac:dyDescent="0.5">
       <c r="A18" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B18" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="E18" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="C18" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="D18" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="E18" s="1" t="s">
+      <c r="F18" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="F18" s="1" t="s">
-        <v>89</v>
-      </c>
       <c r="G18" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H18" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="19" spans="1:8" ht="50.7" x14ac:dyDescent="0.5">
       <c r="A19" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B19" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="E19" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="C19" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="D19" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="E19" s="1" t="s">
+      <c r="F19" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="F19" s="1" t="s">
-        <v>92</v>
-      </c>
       <c r="G19" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H19" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="20" spans="1:8" ht="50.7" x14ac:dyDescent="0.5">
       <c r="A20" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B20" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="E20" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="C20" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="D20" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="E20" s="1" t="s">
+      <c r="F20" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="F20" s="1" t="s">
-        <v>95</v>
-      </c>
       <c r="G20" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H20" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A21" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="B21" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="B21" s="1" t="s">
+      <c r="C21" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="C21" s="1" t="s">
+      <c r="D21" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="D21" s="1" t="s">
-        <v>99</v>
-      </c>
       <c r="E21" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="F21" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="F21" s="1" t="s">
-        <v>79</v>
-      </c>
       <c r="G21" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="H21" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="22" spans="1:8" ht="38" x14ac:dyDescent="0.5">
       <c r="A22" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B22" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="E22" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="C22" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="D22" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="E22" s="1" t="s">
+      <c r="F22" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="F22" s="1" t="s">
-        <v>102</v>
-      </c>
       <c r="G22" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="H22" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="23" spans="1:8" ht="38" x14ac:dyDescent="0.5">
       <c r="A23" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B23" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="E23" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="C23" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="D23" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="E23" s="1" t="s">
+      <c r="F23" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="F23" s="1" t="s">
-        <v>105</v>
-      </c>
       <c r="G23" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H23" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="24" spans="1:8" ht="23.45" customHeight="1" x14ac:dyDescent="0.5"/>

</xml_diff>